<commit_message>
implement sheet drawing in JavaFX
</commit_message>
<xml_diff>
--- a/meja-samples-fx/src/main/resources/com/dua3/meja/fx/samples/test.xlsx
+++ b/meja-samples-fx/src/main/resources/com/dua3/meja/fx/samples/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axelhowind/Projects/meja/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0B73D1-3691-3745-B7F7-51DB459BDC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD11BCC-0E6F-B241-833C-C013B6DB3A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="35800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alignment Test" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="356">
   <si>
     <t>Left</t>
   </si>
@@ -1507,6 +1507,9 @@
   </si>
   <si>
     <t>Distributed (wrap)</t>
+  </si>
+  <si>
+    <t>merged</t>
   </si>
 </sst>
 </file>
@@ -4524,7 +4527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="596">
+  <cellXfs count="597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -5774,15 +5777,6 @@
     <xf numFmtId="0" fontId="0" fillId="389" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="386" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="388" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="389" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="390" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="390" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6012,6 +6006,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="384" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="386" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="388" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="389" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6388,7 +6394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -6402,410 +6408,410 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="569"/>
-      <c r="B1" s="569" t="s">
+      <c r="A1" s="566"/>
+      <c r="B1" s="566" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="570" t="s">
+      <c r="C1" s="567" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="571" t="s">
+      <c r="D1" s="568" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="572" t="s">
+      <c r="E1" s="569" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="573" t="s">
+      <c r="F1" s="570" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="573" t="s">
+      <c r="G1" s="570" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="42.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="574" t="s">
+      <c r="A2" s="571" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="575" t="s">
+      <c r="B2" s="572" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="576" t="s">
+      <c r="C2" s="573" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="577" t="s">
+      <c r="D2" s="574" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="578" t="s">
+      <c r="E2" s="575" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="579" t="s">
+      <c r="F2" s="576" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="579" t="s">
+      <c r="G2" s="576" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="42.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="580" t="s">
+      <c r="A3" s="577" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="581" t="s">
+      <c r="B3" s="578" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="582" t="s">
+      <c r="C3" s="579" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="583" t="s">
+      <c r="D3" s="580" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="584" t="s">
+      <c r="E3" s="581" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="585" t="s">
+      <c r="F3" s="582" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="585" t="s">
+      <c r="G3" s="582" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="42.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="569" t="s">
+      <c r="A4" s="566" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="586" t="s">
+      <c r="B4" s="583" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="587" t="s">
+      <c r="C4" s="584" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="588" t="s">
+      <c r="D4" s="585" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="589" t="s">
+      <c r="E4" s="586" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="590" t="s">
+      <c r="F4" s="587" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="590" t="s">
+      <c r="G4" s="587" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="42.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="569" t="s">
+      <c r="A5" s="566" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="586" t="s">
+      <c r="B5" s="583" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="587" t="s">
+      <c r="C5" s="584" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="588" t="s">
+      <c r="D5" s="585" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="589" t="s">
+      <c r="E5" s="586" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="590" t="s">
+      <c r="F5" s="587" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="590" t="s">
+      <c r="G5" s="587" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="42.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="591" t="s">
+      <c r="A6" s="588" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="592" t="s">
+      <c r="B6" s="589" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="593" t="s">
+      <c r="C6" s="590" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="594" t="s">
+      <c r="D6" s="591" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="595" t="s">
+      <c r="E6" s="592" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="590" t="s">
+      <c r="F6" s="587" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="590" t="s">
+      <c r="G6" s="587" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="543"/>
-      <c r="B8" s="543" t="s">
+      <c r="A8" s="540"/>
+      <c r="B8" s="540" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="544" t="s">
+      <c r="C8" s="541" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="545" t="s">
+      <c r="D8" s="542" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="546" t="s">
+      <c r="E8" s="543" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="547" t="s">
+      <c r="F8" s="544" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="547" t="s">
+      <c r="G8" s="544" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="548" t="s">
+      <c r="A9" s="545" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="549" t="s">
+      <c r="B9" s="546" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="550" t="s">
+      <c r="C9" s="547" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="551" t="s">
+      <c r="D9" s="548" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="552" t="s">
+      <c r="E9" s="549" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="553" t="s">
+      <c r="F9" s="550" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="553" t="s">
+      <c r="G9" s="550" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="554" t="s">
+      <c r="A10" s="551" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="555" t="s">
+      <c r="B10" s="552" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="512" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="556" t="s">
+      <c r="D10" s="553" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="557" t="s">
+      <c r="E10" s="554" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="558" t="s">
+      <c r="F10" s="555" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="558" t="s">
+      <c r="G10" s="555" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="543" t="s">
+      <c r="A11" s="540" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="559" t="s">
+      <c r="B11" s="556" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="560" t="s">
+      <c r="C11" s="557" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="561" t="s">
+      <c r="D11" s="558" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="562" t="s">
+      <c r="E11" s="559" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="563" t="s">
+      <c r="F11" s="560" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="563" t="s">
+      <c r="G11" s="560" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="543" t="s">
+      <c r="A12" s="540" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="559" t="s">
+      <c r="B12" s="556" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="560" t="s">
+      <c r="C12" s="557" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="561" t="s">
+      <c r="D12" s="558" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="562" t="s">
+      <c r="E12" s="559" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="563" t="s">
+      <c r="F12" s="560" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="563" t="s">
+      <c r="G12" s="560" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="564" t="s">
+      <c r="A13" s="561" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="565" t="s">
+      <c r="B13" s="562" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="566" t="s">
+      <c r="C13" s="563" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="567" t="s">
+      <c r="D13" s="564" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="568" t="s">
+      <c r="E13" s="565" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="563" t="s">
+      <c r="F13" s="560" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="563" t="s">
+      <c r="G13" s="560" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="516"/>
-      <c r="B15" s="516" t="s">
+      <c r="A15" s="513"/>
+      <c r="B15" s="513" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="517" t="s">
+      <c r="C15" s="514" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="518" t="s">
+      <c r="D15" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="519" t="s">
+      <c r="E15" s="516" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="520" t="s">
+      <c r="F15" s="517" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="520" t="s">
+      <c r="G15" s="517" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="521" t="s">
+      <c r="A16" s="518" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="522" t="s">
+      <c r="B16" s="519" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="523" t="s">
+      <c r="C16" s="520" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="524" t="s">
+      <c r="D16" s="521" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="525" t="s">
+      <c r="E16" s="522" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="526" t="s">
+      <c r="F16" s="523" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="526" t="s">
+      <c r="G16" s="523" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="527" t="s">
+      <c r="A17" s="524" t="s">
         <v>351</v>
       </c>
-      <c r="B17" s="528" t="s">
+      <c r="B17" s="525" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="529" t="s">
+      <c r="C17" s="526" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="530" t="s">
+      <c r="D17" s="527" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="531" t="s">
+      <c r="E17" s="528" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="532" t="s">
+      <c r="F17" s="529" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="532" t="s">
+      <c r="G17" s="529" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="516" t="s">
+      <c r="A18" s="513" t="s">
         <v>352</v>
       </c>
-      <c r="B18" s="533" t="s">
+      <c r="B18" s="530" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="534" t="s">
+      <c r="C18" s="531" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="535" t="s">
+      <c r="D18" s="532" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="536" t="s">
+      <c r="E18" s="533" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="537" t="s">
+      <c r="F18" s="534" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="537" t="s">
+      <c r="G18" s="534" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="516" t="s">
+      <c r="A19" s="513" t="s">
         <v>353</v>
       </c>
-      <c r="B19" s="533" t="s">
+      <c r="B19" s="530" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="534" t="s">
+      <c r="C19" s="531" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="535" t="s">
+      <c r="D19" s="532" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="536" t="s">
+      <c r="E19" s="533" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="537" t="s">
+      <c r="F19" s="534" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="537" t="s">
+      <c r="G19" s="534" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="100" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="538" t="s">
+      <c r="A20" s="535" t="s">
         <v>354</v>
       </c>
-      <c r="B20" s="539" t="s">
+      <c r="B20" s="536" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="540" t="s">
+      <c r="C20" s="537" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="541" t="s">
+      <c r="D20" s="538" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="542" t="s">
+      <c r="E20" s="539" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="537" t="s">
+      <c r="F20" s="534" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="537" t="s">
+      <c r="G20" s="534" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6823,11 +6829,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9344,19 +9350,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="223" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="513" t="s">
+      <c r="A1" s="593" t="s">
         <v>314</v>
       </c>
-      <c r="B1" s="513"/>
+      <c r="B1" s="593"/>
       <c r="C1" s="417" t="s">
         <v>341</v>
       </c>
@@ -9365,11 +9371,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="514" t="s">
+      <c r="A2" s="594" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="514"/>
-      <c r="C2" s="515" t="s">
+      <c r="B2" s="594"/>
+      <c r="C2" s="595" t="s">
         <v>316</v>
       </c>
       <c r="D2" s="417" t="s">
@@ -9377,16 +9383,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="514"/>
-      <c r="B3" s="514"/>
-      <c r="C3" s="515"/>
+      <c r="A3" s="594"/>
+      <c r="B3" s="594"/>
+      <c r="C3" s="595"/>
       <c r="D3" s="417" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="514"/>
-      <c r="B4" s="514"/>
+      <c r="A4" s="594"/>
+      <c r="B4" s="594"/>
       <c r="C4" s="417" t="s">
         <v>341</v>
       </c>
@@ -9398,10 +9404,10 @@
       <c r="A5" s="417" t="s">
         <v>341</v>
       </c>
-      <c r="B5" s="513" t="s">
+      <c r="B5" s="593" t="s">
         <v>314</v>
       </c>
-      <c r="C5" s="513"/>
+      <c r="C5" s="593"/>
       <c r="D5" s="417" t="s">
         <v>341</v>
       </c>
@@ -9420,12 +9426,21 @@
         <v>341</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="596" t="s">
+        <v>355</v>
+      </c>
+      <c r="B9" s="596"/>
+      <c r="C9" s="596"/>
+      <c r="D9" s="596"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>